<commit_message>
ao: sch-sth kwanza norte update form 2
</commit_message>
<xml_diff>
--- a/SCH-STH/Baseline Mapping/Angola/September 2021/ao_sch_sth_baseline_2_child_kap_202109.xlsx
+++ b/SCH-STH/Baseline Mapping/Angola/September 2021/ao_sch_sth_baseline_2_child_kap_202109.xlsx
@@ -1188,7 +1188,7 @@
     <t>40. Why would you take the medicine to kill intestinal worms (lombrigas) if there is future delivery of medicines in your school to all school children?</t>
   </si>
   <si>
-    <t>40. Ficaste satisfeito com o facto de os professores te terem dado o medicamento para matar as kimbevo ki subisanga omenga (Schistosomíase)?</t>
+    <t>40. Porque tomaria o medicamento para matar os vermes intestinais (lombrigas) se houver uma futura entrega de medicamentos na sua escola a todas as crianças da escola?</t>
   </si>
   <si>
     <t>if(selected(.,'Outros') or selected(.,'7.Nao.sei') or selected(.,'8.Sem.resposta'), count-selected(.)=1, true())</t>
@@ -3457,8 +3457,8 @@
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -3516,7 +3516,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3530,47 +3530,24 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3589,19 +3566,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3629,6 +3605,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -3636,17 +3627,26 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -3677,25 +3677,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3713,19 +3707,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3737,7 +3725,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3749,31 +3827,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3785,61 +3839,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3889,39 +3889,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -3933,6 +3900,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3963,11 +3939,35 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3992,139 +3992,139 @@
     <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -4494,11 +4494,11 @@
   <dimension ref="A1:P175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="K92" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D98" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K125" sqref="K125"/>
+      <selection pane="bottomRight" activeCell="C138" sqref="C138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>

</xml_diff>